<commit_message>
sentence calculator version 1
calculate the length of the sentences in each book
</commit_message>
<xml_diff>
--- a/chapters.xlsx
+++ b/chapters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuxiaoxiao/Documents/电子学校/第二学期/软件大赛备赛/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuxiaoxiao/Text Complex Visulization/Text-Complex-Visulization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6294F6B2-155E-0949-B21A-C5314203CCFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BB37FA-5F1E-7747-9F9F-6D7F1F84FE27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="1460" windowWidth="24140" windowHeight="13080" xr2:uid="{9638D71B-C3FD-3344-894F-802C3B40AB1D}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>第14章</t>
   </si>
   <si>
-    <t>诺伯</t>
-  </si>
-  <si>
     <t>第15章</t>
   </si>
   <si>
@@ -208,6 +205,10 @@
   </si>
   <si>
     <t>第58章</t>
+  </si>
+  <si>
+    <t>chapters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -571,305 +572,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C069F0C6-0A37-6D45-9088-BC975F7E8949}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>